<commit_message>
modificació de la documentació
</commit_message>
<xml_diff>
--- a/documentacion/PlaTreball.xlsx
+++ b/documentacion/PlaTreball.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="75">
   <si>
     <t xml:space="preserve">PLA DE TREBALL</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t xml:space="preserve">Rediseny de llista de obras i usuaris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema d’eliminació d’usuaris Front+Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creació de tablas per als vocabularis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vista d’usuari Backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolució de problema al pujar foto incorrecta</t>
   </si>
 </sst>
 </file>
@@ -916,9 +928,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>929880</xdr:colOff>
+      <xdr:colOff>929520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>721800</xdr:rowOff>
+      <xdr:rowOff>721440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -932,7 +944,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2401200" cy="721800"/>
+          <a:ext cx="2400840" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -958,9 +970,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>929880</xdr:colOff>
+      <xdr:colOff>929520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>721800</xdr:rowOff>
+      <xdr:rowOff>721440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -974,7 +986,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2401200" cy="721800"/>
+          <a:ext cx="2400840" cy="721440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1000,7 +1012,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -1970,10 +1982,10 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -2406,7 +2418,9 @@
       <c r="H25" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="I25" s="29"/>
+      <c r="I25" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="28" t="n">
@@ -2433,7 +2447,9 @@
       <c r="H26" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="I26" s="29"/>
+      <c r="I26" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="n">
@@ -2471,13 +2487,27 @@
       <c r="B28" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="29"/>
+      <c r="C28" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="H28" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" s="29" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="n">
@@ -2486,13 +2516,27 @@
       <c r="B29" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="29"/>
+      <c r="C29" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="n">
@@ -2501,13 +2545,27 @@
       <c r="B30" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="29"/>
+      <c r="C30" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="H30" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" s="29" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="n">
@@ -2516,13 +2574,27 @@
       <c r="B31" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="29"/>
+      <c r="C31" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" s="29" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="n">

</xml_diff>

<commit_message>
Creado diseño de creacion de artwork (no funcional, faltan ajustar SELECTS)
</commit_message>
<xml_diff>
--- a/documentacion/PlaTreball.xlsx
+++ b/documentacion/PlaTreball.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="77">
   <si>
     <t xml:space="preserve">PLA DE TREBALL</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t xml:space="preserve">Resolució de problema al pujar foto incorrecta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creació de progress bar + disseny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Añadida opció de filtrar per estat amb camps de la bdd</t>
   </si>
 </sst>
 </file>
@@ -928,9 +934,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>929520</xdr:colOff>
+      <xdr:colOff>929160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>721440</xdr:rowOff>
+      <xdr:rowOff>721080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -944,7 +950,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2400840" cy="721440"/>
+          <a:ext cx="2400480" cy="721080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -970,9 +976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>929520</xdr:colOff>
+      <xdr:colOff>929160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>721440</xdr:rowOff>
+      <xdr:rowOff>721080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -986,7 +992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2400840" cy="721440"/>
+          <a:ext cx="2400480" cy="721080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1012,7 +1018,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -1981,11 +1987,11 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -2160,7 +2166,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,7 +2224,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="29" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="29" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="29" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,7 +2340,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,7 +2397,9 @@
       <c r="H24" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="29"/>
+      <c r="I24" s="29" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="n">
@@ -2603,13 +2611,27 @@
       <c r="B32" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="29"/>
+      <c r="C32" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H32" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="n">
@@ -2618,13 +2640,27 @@
       <c r="B33" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="29"/>
+      <c r="C33" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="29" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="n">

</xml_diff>

<commit_message>
cambios en el excel de horarios parte 2
</commit_message>
<xml_diff>
--- a/documentacion/PlaTreball.xlsx
+++ b/documentacion/PlaTreball.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="85">
   <si>
     <t xml:space="preserve">PLA DE TREBALL</t>
   </si>
@@ -252,6 +252,30 @@
   </si>
   <si>
     <t xml:space="preserve">Añadida opció de filtrar per estat amb camps de la bdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miguel Ángel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambis en la base de dades i en els models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vista de localitzacions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logica de localitzacions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear localitzacions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vista exposicions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vista crear exposicions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logica crear exposicions</t>
   </si>
 </sst>
 </file>
@@ -934,9 +958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>929160</xdr:colOff>
+      <xdr:colOff>928800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>721080</xdr:rowOff>
+      <xdr:rowOff>720720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -950,7 +974,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2400480" cy="721080"/>
+          <a:ext cx="2400120" cy="720720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -976,9 +1000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>929160</xdr:colOff>
+      <xdr:colOff>928800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>721080</xdr:rowOff>
+      <xdr:rowOff>720720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -992,7 +1016,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2400480" cy="721080"/>
+          <a:ext cx="2400120" cy="720720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1018,7 +1042,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -1988,10 +2012,10 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -2669,13 +2693,27 @@
       <c r="B34" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="29"/>
+      <c r="C34" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="H34" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" s="29" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="n">
@@ -2684,13 +2722,27 @@
       <c r="B35" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="29"/>
+      <c r="C35" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="n">
@@ -2699,13 +2751,27 @@
       <c r="B36" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="29"/>
+      <c r="C36" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="29" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="n">
@@ -2714,13 +2780,131 @@
       <c r="B37" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="29"/>
+      <c r="C37" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="30" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H37" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" s="29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H38" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" s="29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H39" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" s="29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="30" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H40" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" s="29" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H41" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" s="29" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="31" t="s">

</xml_diff>

<commit_message>
Ajustadas horas en excel
</commit_message>
<xml_diff>
--- a/documentacion/PlaTreball.xlsx
+++ b/documentacion/PlaTreball.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="87">
   <si>
     <t xml:space="preserve">PLA DE TREBALL</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t xml:space="preserve">Logica crear exposicions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vista de creacion de obras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vista de modificacion de obras</t>
   </si>
 </sst>
 </file>
@@ -958,9 +964,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>928800</xdr:colOff>
+      <xdr:colOff>928440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>720720</xdr:rowOff>
+      <xdr:rowOff>720360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -974,7 +980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2400120" cy="720720"/>
+          <a:ext cx="2399760" cy="720360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1000,9 +1006,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>928800</xdr:colOff>
+      <xdr:colOff>928440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>720720</xdr:rowOff>
+      <xdr:rowOff>720360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1016,7 +1022,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2400120" cy="720720"/>
+          <a:ext cx="2399760" cy="720360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1042,7 +1048,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -2011,11 +2017,11 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -2803,6 +2809,9 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="28" t="n">
+        <v>23</v>
+      </c>
       <c r="B38" s="28" t="n">
         <v>2</v>
       </c>
@@ -2829,6 +2838,9 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="28" t="n">
+        <v>24</v>
+      </c>
       <c r="B39" s="28" t="n">
         <v>2</v>
       </c>
@@ -2855,6 +2867,9 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="28" t="n">
+        <v>25</v>
+      </c>
       <c r="B40" s="28" t="n">
         <v>2</v>
       </c>
@@ -2881,6 +2896,9 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="28" t="n">
+        <v>26</v>
+      </c>
       <c r="B41" s="28" t="n">
         <v>2</v>
       </c>
@@ -2905,6 +2923,139 @@
       <c r="I41" s="29" t="n">
         <v>2</v>
       </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B42" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H42" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" s="29" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="28" t="n">
+        <v>28</v>
+      </c>
+      <c r="B43" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" s="29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="28" t="n">
+        <v>29</v>
+      </c>
+      <c r="B44" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="29"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="28" t="n">
+        <v>30</v>
+      </c>
+      <c r="B45" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="29"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="28" t="n">
+        <v>31</v>
+      </c>
+      <c r="B46" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="29"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="28" t="n">
+        <v>32</v>
+      </c>
+      <c r="B47" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C47" s="28"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="29"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="28" t="n">
+        <v>33</v>
+      </c>
+      <c r="B48" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="29"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="31" t="s">

</xml_diff>